<commit_message>
update analyse impfungen 2022 herbst
</commit_message>
<xml_diff>
--- a/data/impfungenbooster_standsommer2022.xlsx
+++ b/data/impfungenbooster_standsommer2022.xlsx
@@ -383,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>3120240</v>
+        <v>3123737</v>
       </c>
     </row>
     <row r="3">
@@ -394,7 +394,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>1376658</v>
+        <v>1384544</v>
       </c>
     </row>
     <row r="4">
@@ -405,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>21517</v>
+        <v>23455</v>
       </c>
     </row>
     <row r="5">
@@ -416,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>37210866</v>
+        <v>37224301</v>
       </c>
     </row>
     <row r="6">
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>29333950</v>
+        <v>29399209</v>
       </c>
     </row>
     <row r="7">
@@ -438,7 +438,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1051667</v>
+        <v>1178344</v>
       </c>
     </row>
     <row r="8">
@@ -449,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1052899</v>
+        <v>1057101</v>
       </c>
     </row>
     <row r="9">
@@ -460,7 +460,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>7267</v>
+        <v>7802</v>
       </c>
     </row>
     <row r="10">
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>300</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11">
@@ -482,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>21965709</v>
+        <v>21969674</v>
       </c>
     </row>
     <row r="12">
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>20637892</v>
+        <v>20661882</v>
       </c>
     </row>
     <row r="13">
@@ -504,7 +504,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>5196887</v>
+        <v>5602251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>